<commit_message>
Tesla - Total Revenue, Net Income, Total Assests, Total Liabilities & Cash Flow from Operating Activities extracted from 10-K document for the last 3 financial years
</commit_message>
<xml_diff>
--- a/BCG-GenAI/01_Task_1 - Data_extraction_and_initial_analysis/Task_1_Data_Extraction_&_Initial_Analysis.xlsx
+++ b/BCG-GenAI/01_Task_1 - Data_extraction_and_initial_analysis/Task_1_Data_Extraction_&_Initial_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Forage_Virtual_Internship_Program\BCG-GenAI\01_Task_1 - Data_extraction_and_initial_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C3CE1C-4258-4C96-9614-6A82C3CC304A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACF286C-D6D9-431C-915E-39F80E1F8C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Company</t>
   </si>
@@ -64,6 +64,30 @@
   </si>
   <si>
     <t>Operating Expenses(General &amp; Administrative)</t>
+  </si>
+  <si>
+    <t>81462 </t>
+  </si>
+  <si>
+    <t>53823 </t>
+  </si>
+  <si>
+    <t>3969 </t>
+  </si>
+  <si>
+    <t>3075 </t>
+  </si>
+  <si>
+    <t>2593 </t>
+  </si>
+  <si>
+    <t>4800 </t>
+  </si>
+  <si>
+    <t>3946 </t>
+  </si>
+  <si>
+    <t>4517 </t>
   </si>
 </sst>
 </file>
@@ -107,9 +131,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,7 +420,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,28 +474,28 @@
       <c r="B2">
         <v>2023</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>211915</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>72361</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>411976</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>205753</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>27195</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>22759</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="2">
         <v>7575</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="2">
         <v>57529</v>
       </c>
     </row>
@@ -479,28 +506,28 @@
       <c r="B3">
         <v>2022</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>198270</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>72738</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>364840</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>198298</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>24512</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>21825</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="2">
         <v>5900</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="2">
         <v>52237</v>
       </c>
     </row>
@@ -511,28 +538,28 @@
       <c r="B4">
         <v>2021</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>168088</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>61271</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>333779</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>191791</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>20716</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>20117</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>5107</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
         <v>45940</v>
       </c>
     </row>
@@ -543,6 +570,28 @@
       <c r="B5">
         <v>2023</v>
       </c>
+      <c r="C5" s="2">
+        <v>96773</v>
+      </c>
+      <c r="D5" s="2">
+        <v>14974</v>
+      </c>
+      <c r="E5" s="2">
+        <v>106618</v>
+      </c>
+      <c r="F5" s="2">
+        <v>43009</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -551,6 +600,28 @@
       <c r="B6">
         <v>2022</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2">
+        <v>12587</v>
+      </c>
+      <c r="E6" s="2">
+        <v>82338</v>
+      </c>
+      <c r="F6" s="2">
+        <v>36440</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -559,6 +630,28 @@
       <c r="B7">
         <v>2021</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5644</v>
+      </c>
+      <c r="E7" s="2">
+        <v>62131</v>
+      </c>
+      <c r="F7" s="2">
+        <v>30548</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -567,6 +660,14 @@
       <c r="B8">
         <v>2023</v>
       </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -575,6 +676,14 @@
       <c r="B9">
         <v>2022</v>
       </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -583,6 +692,14 @@
       <c r="B10">
         <v>2021</v>
       </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Apple - Total Revenue, Net Income, Total Assests, Total Liabilities & Cash Flow from Operating Activities extracted from 10-K document for the last 3 financial years
</commit_message>
<xml_diff>
--- a/BCG-GenAI/01_Task_1 - Data_extraction_and_initial_analysis/Task_1_Data_Extraction_&_Initial_Analysis.xlsx
+++ b/BCG-GenAI/01_Task_1 - Data_extraction_and_initial_analysis/Task_1_Data_Extraction_&_Initial_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Forage_Virtual_Internship_Program\BCG-GenAI\01_Task_1 - Data_extraction_and_initial_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACF286C-D6D9-431C-915E-39F80E1F8C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0AD4E0-7C27-4DA3-9E96-C9373982A129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Company</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Total Liabilities (in millions)</t>
   </si>
   <si>
-    <t>Cash Flow from Operating Activities (in millions)</t>
-  </si>
-  <si>
     <t>Microsoft</t>
   </si>
   <si>
@@ -60,34 +57,16 @@
     <t>Operating Expenses(R &amp; D)</t>
   </si>
   <si>
-    <t>Operating Expenses(Sales &amp; Marketing)</t>
-  </si>
-  <si>
-    <t>Operating Expenses(General &amp; Administrative)</t>
-  </si>
-  <si>
     <t>81462 </t>
   </si>
   <si>
     <t>53823 </t>
   </si>
   <si>
-    <t>3969 </t>
-  </si>
-  <si>
-    <t>3075 </t>
-  </si>
-  <si>
-    <t>2593 </t>
-  </si>
-  <si>
-    <t>4800 </t>
-  </si>
-  <si>
-    <t>3946 </t>
-  </si>
-  <si>
-    <t>4517 </t>
+    <t>Operating Expenses(Sales &amp; Marketing, Other Administrative)</t>
+  </si>
+  <si>
+    <t>Total Cash Flow from Operating Activities (in millions)</t>
   </si>
 </sst>
 </file>
@@ -119,7 +98,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -127,14 +106,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -417,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,275 +434,316 @@
     <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="23.88671875" customWidth="1"/>
-    <col min="10" max="10" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C2" s="5">
+        <v>211915</v>
+      </c>
+      <c r="D2" s="5">
+        <v>72361</v>
+      </c>
+      <c r="E2" s="5">
+        <v>411976</v>
+      </c>
+      <c r="F2" s="5">
+        <v>205753</v>
+      </c>
+      <c r="G2" s="5">
+        <v>27195</v>
+      </c>
+      <c r="H2" s="5">
+        <v>30334</v>
+      </c>
+      <c r="I2" s="5">
+        <v>57529</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C3" s="5">
+        <v>198270</v>
+      </c>
+      <c r="D3" s="5">
+        <v>72738</v>
+      </c>
+      <c r="E3" s="5">
+        <v>364840</v>
+      </c>
+      <c r="F3" s="5">
+        <v>198298</v>
+      </c>
+      <c r="G3" s="5">
+        <v>24512</v>
+      </c>
+      <c r="H3" s="5">
+        <v>27725</v>
+      </c>
+      <c r="I3" s="5">
+        <v>52237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C4" s="5">
+        <v>168088</v>
+      </c>
+      <c r="D4" s="5">
+        <v>61271</v>
+      </c>
+      <c r="E4" s="5">
+        <v>333779</v>
+      </c>
+      <c r="F4" s="5">
+        <v>191791</v>
+      </c>
+      <c r="G4" s="5">
+        <v>20716</v>
+      </c>
+      <c r="H4" s="5">
+        <v>25224</v>
+      </c>
+      <c r="I4" s="5">
+        <v>45940</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C5" s="5">
+        <v>96773</v>
+      </c>
+      <c r="D5" s="5">
+        <v>14974</v>
+      </c>
+      <c r="E5" s="5">
+        <v>106618</v>
+      </c>
+      <c r="F5" s="5">
+        <v>43009</v>
+      </c>
+      <c r="G5" s="5">
+        <v>3969</v>
+      </c>
+      <c r="H5" s="5">
+        <v>4800</v>
+      </c>
+      <c r="I5" s="5">
+        <v>8769</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="D6" s="5">
+        <v>12587</v>
+      </c>
+      <c r="E6" s="5">
+        <v>82338</v>
+      </c>
+      <c r="F6" s="5">
+        <v>36440</v>
+      </c>
+      <c r="G6" s="5">
+        <v>3075</v>
+      </c>
+      <c r="H6" s="5">
+        <v>3946</v>
+      </c>
+      <c r="I6" s="5">
+        <v>7021</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
+      <c r="D7" s="5">
+        <v>5644</v>
+      </c>
+      <c r="E7" s="5">
+        <v>62131</v>
+      </c>
+      <c r="F7" s="5">
+        <v>30548</v>
+      </c>
+      <c r="G7" s="5">
+        <v>2593</v>
+      </c>
+      <c r="H7" s="5">
+        <v>4517</v>
+      </c>
+      <c r="I7" s="5">
+        <v>7110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
         <v>2023</v>
       </c>
-      <c r="C2" s="2">
-        <v>211915</v>
-      </c>
-      <c r="D2" s="2">
-        <v>72361</v>
-      </c>
-      <c r="E2" s="2">
-        <v>411976</v>
-      </c>
-      <c r="F2" s="2">
-        <v>205753</v>
-      </c>
-      <c r="G2" s="2">
-        <v>27195</v>
-      </c>
-      <c r="H2" s="2">
-        <v>22759</v>
-      </c>
-      <c r="I2" s="2">
-        <v>7575</v>
-      </c>
-      <c r="J2" s="2">
-        <v>57529</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
+      <c r="C8" s="5">
+        <v>383285</v>
+      </c>
+      <c r="D8" s="5">
+        <v>96995</v>
+      </c>
+      <c r="E8" s="5">
+        <v>352583</v>
+      </c>
+      <c r="F8" s="5">
+        <v>290437</v>
+      </c>
+      <c r="G8" s="5">
+        <v>29915</v>
+      </c>
+      <c r="H8" s="5">
+        <v>24932</v>
+      </c>
+      <c r="I8" s="5">
+        <v>54847</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
         <v>2022</v>
       </c>
-      <c r="C3" s="2">
-        <v>198270</v>
-      </c>
-      <c r="D3" s="2">
-        <v>72738</v>
-      </c>
-      <c r="E3" s="2">
-        <v>364840</v>
-      </c>
-      <c r="F3" s="2">
-        <v>198298</v>
-      </c>
-      <c r="G3" s="2">
-        <v>24512</v>
-      </c>
-      <c r="H3" s="2">
-        <v>21825</v>
-      </c>
-      <c r="I3" s="2">
-        <v>5900</v>
-      </c>
-      <c r="J3" s="2">
-        <v>52237</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
+      <c r="C9" s="5">
+        <v>394328</v>
+      </c>
+      <c r="D9" s="5">
+        <v>99803</v>
+      </c>
+      <c r="E9" s="5">
+        <v>352755</v>
+      </c>
+      <c r="F9" s="5">
+        <v>302083</v>
+      </c>
+      <c r="G9" s="5">
+        <v>26251</v>
+      </c>
+      <c r="H9" s="5">
+        <v>25094</v>
+      </c>
+      <c r="I9" s="5">
+        <v>51345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
         <v>2021</v>
       </c>
-      <c r="C4" s="2">
-        <v>168088</v>
-      </c>
-      <c r="D4" s="2">
-        <v>61271</v>
-      </c>
-      <c r="E4" s="2">
-        <v>333779</v>
-      </c>
-      <c r="F4" s="2">
-        <v>191791</v>
-      </c>
-      <c r="G4" s="2">
-        <v>20716</v>
-      </c>
-      <c r="H4" s="2">
-        <v>20117</v>
-      </c>
-      <c r="I4" s="2">
-        <v>5107</v>
-      </c>
-      <c r="J4" s="2">
-        <v>45940</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>2023</v>
-      </c>
-      <c r="C5" s="2">
-        <v>96773</v>
-      </c>
-      <c r="D5" s="2">
-        <v>14974</v>
-      </c>
-      <c r="E5" s="2">
-        <v>106618</v>
-      </c>
-      <c r="F5" s="2">
-        <v>43009</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>2022</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2">
-        <v>12587</v>
-      </c>
-      <c r="E6" s="2">
-        <v>82338</v>
-      </c>
-      <c r="F6" s="2">
-        <v>36440</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>2021</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="2">
-        <v>5644</v>
-      </c>
-      <c r="E7" s="2">
-        <v>62131</v>
-      </c>
-      <c r="F7" s="2">
-        <v>30548</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>2023</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>2022</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>2021</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="C10" s="5">
+        <v>365817</v>
+      </c>
+      <c r="D10" s="5">
+        <v>94680</v>
+      </c>
+      <c r="E10" s="5">
+        <v>351002</v>
+      </c>
+      <c r="F10" s="5">
+        <v>287912</v>
+      </c>
+      <c r="G10" s="5">
+        <v>21914</v>
+      </c>
+      <c r="H10" s="5">
+        <v>21973</v>
+      </c>
+      <c r="I10" s="5">
+        <v>43887</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>